<commit_message>
updated country ref to fix mispelling in Japan.
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Country Reference.xlsx
+++ b/mppsteel/data/import_data/Country Reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="531" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF69F6FC-EABA-45F1-AA6C-B7FA64A28BA4}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB39D86-AA5D-46B1-9DA8-FA665A72CE5A}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{399614B1-7431-4F70-9F99-85E1D48DE75C}"/>
   </bookViews>
@@ -858,9 +858,6 @@
     <t>JPN</t>
   </si>
   <si>
-    <t>Japan. South Korea, and Taiwan</t>
-  </si>
-  <si>
     <t>Jersey</t>
   </si>
   <si>
@@ -1675,6 +1672,9 @@
   </si>
   <si>
     <t>Sint Maarten</t>
+  </si>
+  <si>
+    <t>Japan, South Korea, and Taiwan</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2054,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2203,7 +2203,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -2295,7 +2295,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -2410,7 +2410,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -2525,7 +2525,7 @@
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
@@ -2686,12 +2686,12 @@
         <v>11</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B28" t="s">
         <v>86</v>
@@ -2893,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
@@ -3008,7 +3008,7 @@
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
@@ -3238,7 +3238,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
@@ -3261,7 +3261,7 @@
         <v>27</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
@@ -3353,7 +3353,7 @@
         <v>27</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.5">
@@ -3537,7 +3537,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.5">
@@ -3841,7 +3841,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B78" t="s">
         <v>191</v>
@@ -3905,7 +3905,7 @@
         <v>27</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.5">
@@ -3997,7 +3997,7 @@
         <v>27</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.5">
@@ -4020,7 +4020,7 @@
         <v>23</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.5">
@@ -4089,7 +4089,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.5">
@@ -4204,7 +4204,7 @@
         <v>37</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.5">
@@ -4273,7 +4273,7 @@
         <v>27</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.5">
@@ -4434,7 +4434,7 @@
         <v>27</v>
       </c>
       <c r="G103" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.5">
@@ -4572,7 +4572,7 @@
         <v>11</v>
       </c>
       <c r="G109" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.5">
@@ -4687,7 +4687,7 @@
         <v>11</v>
       </c>
       <c r="G114" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.5">
@@ -4756,15 +4756,15 @@
         <v>271</v>
       </c>
       <c r="G117" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A118" t="s">
+        <v>273</v>
+      </c>
+      <c r="B118" t="s">
         <v>274</v>
-      </c>
-      <c r="B118" t="s">
-        <v>275</v>
       </c>
       <c r="C118">
         <v>832</v>
@@ -4784,10 +4784,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A119" t="s">
+        <v>275</v>
+      </c>
+      <c r="B119" t="s">
         <v>276</v>
-      </c>
-      <c r="B119" t="s">
-        <v>277</v>
       </c>
       <c r="C119">
         <v>400</v>
@@ -4802,21 +4802,21 @@
         <v>11</v>
       </c>
       <c r="G119" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
+        <v>278</v>
+      </c>
+      <c r="B120" t="s">
         <v>279</v>
-      </c>
-      <c r="B120" t="s">
-        <v>280</v>
       </c>
       <c r="C120">
         <v>398</v>
       </c>
       <c r="D120" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E120" t="s">
         <v>10</v>
@@ -4830,10 +4830,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
+        <v>281</v>
+      </c>
+      <c r="B121" t="s">
         <v>282</v>
-      </c>
-      <c r="B121" t="s">
-        <v>283</v>
       </c>
       <c r="C121">
         <v>404</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
+        <v>283</v>
+      </c>
+      <c r="B122" t="s">
         <v>284</v>
-      </c>
-      <c r="B122" t="s">
-        <v>285</v>
       </c>
       <c r="C122">
         <v>296</v>
@@ -4871,15 +4871,15 @@
         <v>27</v>
       </c>
       <c r="G122" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
+        <v>285</v>
+      </c>
+      <c r="B123" t="s">
         <v>286</v>
-      </c>
-      <c r="B123" t="s">
-        <v>287</v>
       </c>
       <c r="C123">
         <v>414</v>
@@ -4899,16 +4899,16 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
+        <v>287</v>
+      </c>
+      <c r="B124" t="s">
         <v>288</v>
-      </c>
-      <c r="B124" t="s">
-        <v>289</v>
       </c>
       <c r="C124">
         <v>417</v>
       </c>
       <c r="D124" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -4922,10 +4922,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
+        <v>289</v>
+      </c>
+      <c r="B125" t="s">
         <v>290</v>
-      </c>
-      <c r="B125" t="s">
-        <v>291</v>
       </c>
       <c r="C125">
         <v>418</v>
@@ -4940,15 +4940,15 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
+        <v>291</v>
+      </c>
+      <c r="B126" t="s">
         <v>292</v>
-      </c>
-      <c r="B126" t="s">
-        <v>293</v>
       </c>
       <c r="C126">
         <v>428</v>
@@ -4968,10 +4968,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
+        <v>293</v>
+      </c>
+      <c r="B127" t="s">
         <v>294</v>
-      </c>
-      <c r="B127" t="s">
-        <v>295</v>
       </c>
       <c r="C127">
         <v>422</v>
@@ -4991,10 +4991,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
+        <v>295</v>
+      </c>
+      <c r="B128" t="s">
         <v>296</v>
-      </c>
-      <c r="B128" t="s">
-        <v>297</v>
       </c>
       <c r="C128">
         <v>426</v>
@@ -5014,10 +5014,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A129" t="s">
+        <v>297</v>
+      </c>
+      <c r="B129" t="s">
         <v>298</v>
-      </c>
-      <c r="B129" t="s">
-        <v>299</v>
       </c>
       <c r="C129">
         <v>430</v>
@@ -5037,10 +5037,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
+        <v>299</v>
+      </c>
+      <c r="B130" t="s">
         <v>300</v>
-      </c>
-      <c r="B130" t="s">
-        <v>301</v>
       </c>
       <c r="C130">
         <v>434</v>
@@ -5060,10 +5060,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A131" t="s">
+        <v>301</v>
+      </c>
+      <c r="B131" t="s">
         <v>302</v>
-      </c>
-      <c r="B131" t="s">
-        <v>303</v>
       </c>
       <c r="C131">
         <v>438</v>
@@ -5083,10 +5083,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A132" t="s">
+        <v>303</v>
+      </c>
+      <c r="B132" t="s">
         <v>304</v>
-      </c>
-      <c r="B132" t="s">
-        <v>305</v>
       </c>
       <c r="C132">
         <v>440</v>
@@ -5106,10 +5106,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A133" t="s">
+        <v>305</v>
+      </c>
+      <c r="B133" t="s">
         <v>306</v>
-      </c>
-      <c r="B133" t="s">
-        <v>307</v>
       </c>
       <c r="C133">
         <v>442</v>
@@ -5129,10 +5129,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
+        <v>307</v>
+      </c>
+      <c r="B134" t="s">
         <v>308</v>
-      </c>
-      <c r="B134" t="s">
-        <v>309</v>
       </c>
       <c r="C134">
         <v>450</v>
@@ -5152,10 +5152,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A135" t="s">
+        <v>309</v>
+      </c>
+      <c r="B135" t="s">
         <v>310</v>
-      </c>
-      <c r="B135" t="s">
-        <v>311</v>
       </c>
       <c r="C135">
         <v>454</v>
@@ -5175,10 +5175,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A136" t="s">
+        <v>311</v>
+      </c>
+      <c r="B136" t="s">
         <v>312</v>
-      </c>
-      <c r="B136" t="s">
-        <v>313</v>
       </c>
       <c r="C136">
         <v>458</v>
@@ -5193,15 +5193,15 @@
         <v>11</v>
       </c>
       <c r="G136" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A137" t="s">
+        <v>313</v>
+      </c>
+      <c r="B137" t="s">
         <v>314</v>
-      </c>
-      <c r="B137" t="s">
-        <v>315</v>
       </c>
       <c r="C137">
         <v>462</v>
@@ -5216,15 +5216,15 @@
         <v>11</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
+        <v>315</v>
+      </c>
+      <c r="B138" t="s">
         <v>316</v>
-      </c>
-      <c r="B138" t="s">
-        <v>317</v>
       </c>
       <c r="C138">
         <v>466</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A139" t="s">
+        <v>317</v>
+      </c>
+      <c r="B139" t="s">
         <v>318</v>
-      </c>
-      <c r="B139" t="s">
-        <v>319</v>
       </c>
       <c r="C139">
         <v>470</v>
@@ -5267,10 +5267,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A140" t="s">
+        <v>319</v>
+      </c>
+      <c r="B140" t="s">
         <v>320</v>
-      </c>
-      <c r="B140" t="s">
-        <v>321</v>
       </c>
       <c r="C140">
         <v>584</v>
@@ -5285,15 +5285,15 @@
         <v>27</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A141" t="s">
+        <v>321</v>
+      </c>
+      <c r="B141" t="s">
         <v>322</v>
-      </c>
-      <c r="B141" t="s">
-        <v>323</v>
       </c>
       <c r="C141">
         <v>474</v>
@@ -5313,10 +5313,10 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A142" t="s">
+        <v>323</v>
+      </c>
+      <c r="B142" t="s">
         <v>324</v>
-      </c>
-      <c r="B142" t="s">
-        <v>325</v>
       </c>
       <c r="C142">
         <v>478</v>
@@ -5336,10 +5336,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A143" t="s">
+        <v>325</v>
+      </c>
+      <c r="B143" t="s">
         <v>326</v>
-      </c>
-      <c r="B143" t="s">
-        <v>327</v>
       </c>
       <c r="C143">
         <v>480</v>
@@ -5359,10 +5359,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A144" t="s">
+        <v>327</v>
+      </c>
+      <c r="B144" t="s">
         <v>328</v>
-      </c>
-      <c r="B144" t="s">
-        <v>329</v>
       </c>
       <c r="C144">
         <v>175</v>
@@ -5382,10 +5382,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A145" t="s">
+        <v>329</v>
+      </c>
+      <c r="B145" t="s">
         <v>330</v>
-      </c>
-      <c r="B145" t="s">
-        <v>331</v>
       </c>
       <c r="C145">
         <v>484</v>
@@ -5405,10 +5405,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A146" t="s">
+        <v>331</v>
+      </c>
+      <c r="B146" t="s">
         <v>332</v>
-      </c>
-      <c r="B146" t="s">
-        <v>333</v>
       </c>
       <c r="C146">
         <v>583</v>
@@ -5423,15 +5423,15 @@
         <v>27</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A147" t="s">
+        <v>333</v>
+      </c>
+      <c r="B147" t="s">
         <v>334</v>
-      </c>
-      <c r="B147" t="s">
-        <v>335</v>
       </c>
       <c r="C147">
         <v>492</v>
@@ -5451,10 +5451,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A148" t="s">
+        <v>335</v>
+      </c>
+      <c r="B148" t="s">
         <v>336</v>
-      </c>
-      <c r="B148" t="s">
-        <v>337</v>
       </c>
       <c r="C148">
         <v>496</v>
@@ -5469,15 +5469,15 @@
         <v>11</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A149" t="s">
+        <v>337</v>
+      </c>
+      <c r="B149" t="s">
         <v>338</v>
-      </c>
-      <c r="B149" t="s">
-        <v>339</v>
       </c>
       <c r="C149">
         <v>499</v>
@@ -5497,10 +5497,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A150" t="s">
+        <v>339</v>
+      </c>
+      <c r="B150" t="s">
         <v>340</v>
-      </c>
-      <c r="B150" t="s">
-        <v>341</v>
       </c>
       <c r="C150">
         <v>500</v>
@@ -5520,10 +5520,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A151" t="s">
+        <v>341</v>
+      </c>
+      <c r="B151" t="s">
         <v>342</v>
-      </c>
-      <c r="B151" t="s">
-        <v>343</v>
       </c>
       <c r="C151">
         <v>504</v>
@@ -5543,10 +5543,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A152" t="s">
+        <v>343</v>
+      </c>
+      <c r="B152" t="s">
         <v>344</v>
-      </c>
-      <c r="B152" t="s">
-        <v>345</v>
       </c>
       <c r="C152">
         <v>508</v>
@@ -5566,10 +5566,10 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A153" t="s">
+        <v>345</v>
+      </c>
+      <c r="B153" t="s">
         <v>346</v>
-      </c>
-      <c r="B153" t="s">
-        <v>347</v>
       </c>
       <c r="C153">
         <v>104</v>
@@ -5584,15 +5584,15 @@
         <v>11</v>
       </c>
       <c r="G153" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A154" t="s">
+        <v>347</v>
+      </c>
+      <c r="B154" t="s">
         <v>348</v>
-      </c>
-      <c r="B154" t="s">
-        <v>349</v>
       </c>
       <c r="C154">
         <v>516</v>
@@ -5612,10 +5612,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A155" t="s">
+        <v>349</v>
+      </c>
+      <c r="B155" t="s">
         <v>350</v>
-      </c>
-      <c r="B155" t="s">
-        <v>351</v>
       </c>
       <c r="C155">
         <v>520</v>
@@ -5630,15 +5630,15 @@
         <v>27</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A156" t="s">
+        <v>351</v>
+      </c>
+      <c r="B156" t="s">
         <v>352</v>
-      </c>
-      <c r="B156" t="s">
-        <v>353</v>
       </c>
       <c r="C156">
         <v>524</v>
@@ -5653,15 +5653,15 @@
         <v>11</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A157" t="s">
+        <v>353</v>
+      </c>
+      <c r="B157" t="s">
         <v>354</v>
-      </c>
-      <c r="B157" t="s">
-        <v>355</v>
       </c>
       <c r="C157">
         <v>528</v>
@@ -5681,10 +5681,10 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A158" t="s">
+        <v>355</v>
+      </c>
+      <c r="B158" t="s">
         <v>356</v>
-      </c>
-      <c r="B158" t="s">
-        <v>357</v>
       </c>
       <c r="C158">
         <v>540</v>
@@ -5699,15 +5699,15 @@
         <v>27</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A159" t="s">
+        <v>357</v>
+      </c>
+      <c r="B159" t="s">
         <v>358</v>
-      </c>
-      <c r="B159" t="s">
-        <v>359</v>
       </c>
       <c r="C159">
         <v>554</v>
@@ -5722,15 +5722,15 @@
         <v>27</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A160" t="s">
+        <v>359</v>
+      </c>
+      <c r="B160" t="s">
         <v>360</v>
-      </c>
-      <c r="B160" t="s">
-        <v>361</v>
       </c>
       <c r="C160">
         <v>558</v>
@@ -5750,10 +5750,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A161" t="s">
+        <v>361</v>
+      </c>
+      <c r="B161" t="s">
         <v>362</v>
-      </c>
-      <c r="B161" t="s">
-        <v>363</v>
       </c>
       <c r="C161">
         <v>562</v>
@@ -5773,10 +5773,10 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A162" t="s">
+        <v>363</v>
+      </c>
+      <c r="B162" t="s">
         <v>364</v>
-      </c>
-      <c r="B162" t="s">
-        <v>365</v>
       </c>
       <c r="C162">
         <v>566</v>
@@ -5796,10 +5796,10 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A163" t="s">
+        <v>365</v>
+      </c>
+      <c r="B163" t="s">
         <v>366</v>
-      </c>
-      <c r="B163" t="s">
-        <v>367</v>
       </c>
       <c r="C163">
         <v>570</v>
@@ -5814,15 +5814,15 @@
         <v>27</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A164" t="s">
+        <v>367</v>
+      </c>
+      <c r="B164" t="s">
         <v>368</v>
-      </c>
-      <c r="B164" t="s">
-        <v>369</v>
       </c>
       <c r="C164">
         <v>574</v>
@@ -5837,15 +5837,15 @@
         <v>27</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A165" t="s">
+        <v>369</v>
+      </c>
+      <c r="B165" t="s">
         <v>370</v>
-      </c>
-      <c r="B165" t="s">
-        <v>371</v>
       </c>
       <c r="C165">
         <v>807</v>
@@ -5865,10 +5865,10 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A166" t="s">
+        <v>371</v>
+      </c>
+      <c r="B166" t="s">
         <v>372</v>
-      </c>
-      <c r="B166" t="s">
-        <v>373</v>
       </c>
       <c r="C166">
         <v>580</v>
@@ -5883,15 +5883,15 @@
         <v>27</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A167" t="s">
+        <v>373</v>
+      </c>
+      <c r="B167" t="s">
         <v>374</v>
-      </c>
-      <c r="B167" t="s">
-        <v>375</v>
       </c>
       <c r="C167">
         <v>578</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A168" t="s">
+        <v>375</v>
+      </c>
+      <c r="B168" t="s">
         <v>376</v>
-      </c>
-      <c r="B168" t="s">
-        <v>377</v>
       </c>
       <c r="C168">
         <v>512</v>
@@ -5934,10 +5934,10 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A169" t="s">
+        <v>377</v>
+      </c>
+      <c r="B169" t="s">
         <v>378</v>
-      </c>
-      <c r="B169" t="s">
-        <v>379</v>
       </c>
       <c r="C169">
         <v>586</v>
@@ -5952,15 +5952,15 @@
         <v>11</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A170" t="s">
+        <v>379</v>
+      </c>
+      <c r="B170" t="s">
         <v>380</v>
-      </c>
-      <c r="B170" t="s">
-        <v>381</v>
       </c>
       <c r="C170">
         <v>585</v>
@@ -5975,15 +5975,15 @@
         <v>27</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A171" t="s">
+        <v>381</v>
+      </c>
+      <c r="B171" t="s">
         <v>382</v>
-      </c>
-      <c r="B171" t="s">
-        <v>383</v>
       </c>
       <c r="C171">
         <v>591</v>
@@ -6003,10 +6003,10 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A172" t="s">
+        <v>383</v>
+      </c>
+      <c r="B172" t="s">
         <v>384</v>
-      </c>
-      <c r="B172" t="s">
-        <v>385</v>
       </c>
       <c r="C172">
         <v>598</v>
@@ -6021,15 +6021,15 @@
         <v>27</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A173" t="s">
+        <v>385</v>
+      </c>
+      <c r="B173" t="s">
         <v>386</v>
-      </c>
-      <c r="B173" t="s">
-        <v>387</v>
       </c>
       <c r="C173">
         <v>600</v>
@@ -6049,10 +6049,10 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A174" t="s">
+        <v>387</v>
+      </c>
+      <c r="B174" t="s">
         <v>388</v>
-      </c>
-      <c r="B174" t="s">
-        <v>389</v>
       </c>
       <c r="C174">
         <v>604</v>
@@ -6072,10 +6072,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A175" t="s">
+        <v>389</v>
+      </c>
+      <c r="B175" t="s">
         <v>390</v>
-      </c>
-      <c r="B175" t="s">
-        <v>391</v>
       </c>
       <c r="C175">
         <v>608</v>
@@ -6090,15 +6090,15 @@
         <v>11</v>
       </c>
       <c r="G175" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A176" t="s">
+        <v>391</v>
+      </c>
+      <c r="B176" t="s">
         <v>392</v>
-      </c>
-      <c r="B176" t="s">
-        <v>393</v>
       </c>
       <c r="C176">
         <v>612</v>
@@ -6113,15 +6113,15 @@
         <v>27</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A177" t="s">
+        <v>393</v>
+      </c>
+      <c r="B177" t="s">
         <v>394</v>
-      </c>
-      <c r="B177" t="s">
-        <v>395</v>
       </c>
       <c r="C177">
         <v>616</v>
@@ -6141,10 +6141,10 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A178" t="s">
+        <v>395</v>
+      </c>
+      <c r="B178" t="s">
         <v>396</v>
-      </c>
-      <c r="B178" t="s">
-        <v>397</v>
       </c>
       <c r="C178">
         <v>620</v>
@@ -6164,10 +6164,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A179" t="s">
+        <v>397</v>
+      </c>
+      <c r="B179" t="s">
         <v>398</v>
-      </c>
-      <c r="B179" t="s">
-        <v>399</v>
       </c>
       <c r="C179">
         <v>630</v>
@@ -6187,10 +6187,10 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A180" t="s">
+        <v>399</v>
+      </c>
+      <c r="B180" t="s">
         <v>400</v>
-      </c>
-      <c r="B180" t="s">
-        <v>401</v>
       </c>
       <c r="C180">
         <v>634</v>
@@ -6210,10 +6210,10 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A181" t="s">
+        <v>401</v>
+      </c>
+      <c r="B181" t="s">
         <v>402</v>
-      </c>
-      <c r="B181" t="s">
-        <v>403</v>
       </c>
       <c r="C181">
         <v>410</v>
@@ -6228,15 +6228,15 @@
         <v>11</v>
       </c>
       <c r="G181" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A182" t="s">
+        <v>403</v>
+      </c>
+      <c r="B182" t="s">
         <v>404</v>
-      </c>
-      <c r="B182" t="s">
-        <v>405</v>
       </c>
       <c r="C182">
         <v>498</v>
@@ -6256,10 +6256,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A183" t="s">
+        <v>405</v>
+      </c>
+      <c r="B183" t="s">
         <v>406</v>
-      </c>
-      <c r="B183" t="s">
-        <v>407</v>
       </c>
       <c r="C183">
         <v>638</v>
@@ -6279,10 +6279,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A184" t="s">
+        <v>407</v>
+      </c>
+      <c r="B184" t="s">
         <v>408</v>
-      </c>
-      <c r="B184" t="s">
-        <v>409</v>
       </c>
       <c r="C184">
         <v>642</v>
@@ -6302,10 +6302,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A185" t="s">
+        <v>409</v>
+      </c>
+      <c r="B185" t="s">
         <v>410</v>
-      </c>
-      <c r="B185" t="s">
-        <v>411</v>
       </c>
       <c r="C185">
         <v>643</v>
@@ -6325,10 +6325,10 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A186" t="s">
+        <v>411</v>
+      </c>
+      <c r="B186" t="s">
         <v>412</v>
-      </c>
-      <c r="B186" t="s">
-        <v>413</v>
       </c>
       <c r="C186">
         <v>646</v>
@@ -6348,10 +6348,10 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A187" t="s">
+        <v>413</v>
+      </c>
+      <c r="B187" t="s">
         <v>414</v>
-      </c>
-      <c r="B187" t="s">
-        <v>415</v>
       </c>
       <c r="C187">
         <v>652</v>
@@ -6371,10 +6371,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A188" t="s">
+        <v>415</v>
+      </c>
+      <c r="B188" t="s">
         <v>416</v>
-      </c>
-      <c r="B188" t="s">
-        <v>417</v>
       </c>
       <c r="C188">
         <v>654</v>
@@ -6389,15 +6389,15 @@
         <v>23</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A189" t="s">
+        <v>417</v>
+      </c>
+      <c r="B189" t="s">
         <v>418</v>
-      </c>
-      <c r="B189" t="s">
-        <v>419</v>
       </c>
       <c r="C189">
         <v>659</v>
@@ -6417,10 +6417,10 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A190" t="s">
+        <v>419</v>
+      </c>
+      <c r="B190" t="s">
         <v>420</v>
-      </c>
-      <c r="B190" t="s">
-        <v>421</v>
       </c>
       <c r="C190">
         <v>662</v>
@@ -6440,10 +6440,10 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A191" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B191" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C191">
         <v>663</v>
@@ -6463,10 +6463,10 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A192" t="s">
+        <v>422</v>
+      </c>
+      <c r="B192" t="s">
         <v>423</v>
-      </c>
-      <c r="B192" t="s">
-        <v>424</v>
       </c>
       <c r="C192">
         <v>666</v>
@@ -6486,10 +6486,10 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A193" t="s">
+        <v>424</v>
+      </c>
+      <c r="B193" t="s">
         <v>425</v>
-      </c>
-      <c r="B193" t="s">
-        <v>426</v>
       </c>
       <c r="C193">
         <v>670</v>
@@ -6509,10 +6509,10 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A194" t="s">
+        <v>426</v>
+      </c>
+      <c r="B194" t="s">
         <v>427</v>
-      </c>
-      <c r="B194" t="s">
-        <v>428</v>
       </c>
       <c r="C194">
         <v>882</v>
@@ -6527,15 +6527,15 @@
         <v>27</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A195" t="s">
+        <v>428</v>
+      </c>
+      <c r="B195" t="s">
         <v>429</v>
-      </c>
-      <c r="B195" t="s">
-        <v>430</v>
       </c>
       <c r="C195">
         <v>674</v>
@@ -6555,10 +6555,10 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A196" t="s">
+        <v>430</v>
+      </c>
+      <c r="B196" t="s">
         <v>431</v>
-      </c>
-      <c r="B196" t="s">
-        <v>432</v>
       </c>
       <c r="C196">
         <v>678</v>
@@ -6578,10 +6578,10 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A197" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B197" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C197">
         <v>680</v>
@@ -6601,10 +6601,10 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A198" t="s">
+        <v>433</v>
+      </c>
+      <c r="B198" t="s">
         <v>434</v>
-      </c>
-      <c r="B198" t="s">
-        <v>435</v>
       </c>
       <c r="C198">
         <v>682</v>
@@ -6624,10 +6624,10 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A199" t="s">
+        <v>435</v>
+      </c>
+      <c r="B199" t="s">
         <v>436</v>
-      </c>
-      <c r="B199" t="s">
-        <v>437</v>
       </c>
       <c r="C199">
         <v>686</v>
@@ -6647,10 +6647,10 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A200" t="s">
+        <v>437</v>
+      </c>
+      <c r="B200" t="s">
         <v>438</v>
-      </c>
-      <c r="B200" t="s">
-        <v>439</v>
       </c>
       <c r="C200">
         <v>688</v>
@@ -6670,10 +6670,10 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A201" t="s">
+        <v>439</v>
+      </c>
+      <c r="B201" t="s">
         <v>440</v>
-      </c>
-      <c r="B201" t="s">
-        <v>441</v>
       </c>
       <c r="C201">
         <v>690</v>
@@ -6688,15 +6688,15 @@
         <v>23</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A202" t="s">
+        <v>441</v>
+      </c>
+      <c r="B202" t="s">
         <v>442</v>
-      </c>
-      <c r="B202" t="s">
-        <v>443</v>
       </c>
       <c r="C202">
         <v>694</v>
@@ -6716,10 +6716,10 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A203" t="s">
+        <v>443</v>
+      </c>
+      <c r="B203" t="s">
         <v>444</v>
-      </c>
-      <c r="B203" t="s">
-        <v>445</v>
       </c>
       <c r="C203">
         <v>702</v>
@@ -6734,15 +6734,15 @@
         <v>11</v>
       </c>
       <c r="G203" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A204" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B204" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C204">
         <v>534</v>
@@ -6757,15 +6757,15 @@
         <v>37</v>
       </c>
       <c r="G204" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A205" t="s">
+        <v>446</v>
+      </c>
+      <c r="B205" t="s">
         <v>447</v>
-      </c>
-      <c r="B205" t="s">
-        <v>448</v>
       </c>
       <c r="C205">
         <v>703</v>
@@ -6785,10 +6785,10 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A206" t="s">
+        <v>448</v>
+      </c>
+      <c r="B206" t="s">
         <v>449</v>
-      </c>
-      <c r="B206" t="s">
-        <v>450</v>
       </c>
       <c r="C206">
         <v>705</v>
@@ -6808,10 +6808,10 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A207" t="s">
+        <v>450</v>
+      </c>
+      <c r="B207" t="s">
         <v>451</v>
-      </c>
-      <c r="B207" t="s">
-        <v>452</v>
       </c>
       <c r="C207">
         <v>90</v>
@@ -6826,15 +6826,15 @@
         <v>27</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A208" t="s">
+        <v>452</v>
+      </c>
+      <c r="B208" t="s">
         <v>453</v>
-      </c>
-      <c r="B208" t="s">
-        <v>454</v>
       </c>
       <c r="C208">
         <v>706</v>
@@ -6854,10 +6854,10 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A209" t="s">
+        <v>454</v>
+      </c>
+      <c r="B209" t="s">
         <v>455</v>
-      </c>
-      <c r="B209" t="s">
-        <v>456</v>
       </c>
       <c r="C209">
         <v>710</v>
@@ -6877,10 +6877,10 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A210" t="s">
+        <v>456</v>
+      </c>
+      <c r="B210" t="s">
         <v>457</v>
-      </c>
-      <c r="B210" t="s">
-        <v>458</v>
       </c>
       <c r="C210">
         <v>239</v>
@@ -6900,10 +6900,10 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A211" t="s">
+        <v>458</v>
+      </c>
+      <c r="B211" t="s">
         <v>459</v>
-      </c>
-      <c r="B211" t="s">
-        <v>460</v>
       </c>
       <c r="C211">
         <v>728</v>
@@ -6923,10 +6923,10 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A212" t="s">
+        <v>460</v>
+      </c>
+      <c r="B212" t="s">
         <v>461</v>
-      </c>
-      <c r="B212" t="s">
-        <v>462</v>
       </c>
       <c r="C212">
         <v>724</v>
@@ -6946,10 +6946,10 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A213" t="s">
+        <v>462</v>
+      </c>
+      <c r="B213" t="s">
         <v>463</v>
-      </c>
-      <c r="B213" t="s">
-        <v>464</v>
       </c>
       <c r="C213">
         <v>144</v>
@@ -6964,15 +6964,15 @@
         <v>11</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A214" t="s">
+        <v>464</v>
+      </c>
+      <c r="B214" t="s">
         <v>465</v>
-      </c>
-      <c r="B214" t="s">
-        <v>466</v>
       </c>
       <c r="C214">
         <v>275</v>
@@ -6992,10 +6992,10 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A215" t="s">
+        <v>466</v>
+      </c>
+      <c r="B215" t="s">
         <v>467</v>
-      </c>
-      <c r="B215" t="s">
-        <v>468</v>
       </c>
       <c r="C215">
         <v>729</v>
@@ -7015,10 +7015,10 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A216" t="s">
+        <v>468</v>
+      </c>
+      <c r="B216" t="s">
         <v>469</v>
-      </c>
-      <c r="B216" t="s">
-        <v>470</v>
       </c>
       <c r="C216">
         <v>740</v>
@@ -7038,10 +7038,10 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A217" t="s">
+        <v>470</v>
+      </c>
+      <c r="B217" t="s">
         <v>471</v>
-      </c>
-      <c r="B217" t="s">
-        <v>472</v>
       </c>
       <c r="C217">
         <v>744</v>
@@ -7061,10 +7061,10 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A218" t="s">
+        <v>472</v>
+      </c>
+      <c r="B218" t="s">
         <v>473</v>
-      </c>
-      <c r="B218" t="s">
-        <v>474</v>
       </c>
       <c r="C218">
         <v>752</v>
@@ -7084,10 +7084,10 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A219" t="s">
+        <v>474</v>
+      </c>
+      <c r="B219" t="s">
         <v>475</v>
-      </c>
-      <c r="B219" t="s">
-        <v>476</v>
       </c>
       <c r="C219">
         <v>756</v>
@@ -7107,10 +7107,10 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A220" t="s">
+        <v>476</v>
+      </c>
+      <c r="B220" t="s">
         <v>477</v>
-      </c>
-      <c r="B220" t="s">
-        <v>478</v>
       </c>
       <c r="C220">
         <v>760</v>
@@ -7130,16 +7130,16 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A221" t="s">
+        <v>478</v>
+      </c>
+      <c r="B221" t="s">
         <v>479</v>
-      </c>
-      <c r="B221" t="s">
-        <v>480</v>
       </c>
       <c r="C221">
         <v>762</v>
       </c>
       <c r="D221" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E221" t="s">
         <v>10</v>
@@ -7153,10 +7153,10 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A222" t="s">
+        <v>480</v>
+      </c>
+      <c r="B222" t="s">
         <v>481</v>
-      </c>
-      <c r="B222" t="s">
-        <v>482</v>
       </c>
       <c r="C222">
         <v>764</v>
@@ -7171,15 +7171,15 @@
         <v>11</v>
       </c>
       <c r="G222" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A223" t="s">
+        <v>482</v>
+      </c>
+      <c r="B223" t="s">
         <v>483</v>
-      </c>
-      <c r="B223" t="s">
-        <v>484</v>
       </c>
       <c r="C223">
         <v>626</v>
@@ -7194,15 +7194,15 @@
         <v>11</v>
       </c>
       <c r="G223" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A224" t="s">
+        <v>484</v>
+      </c>
+      <c r="B224" t="s">
         <v>485</v>
-      </c>
-      <c r="B224" t="s">
-        <v>486</v>
       </c>
       <c r="C224">
         <v>768</v>
@@ -7222,10 +7222,10 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A225" t="s">
+        <v>486</v>
+      </c>
+      <c r="B225" t="s">
         <v>487</v>
-      </c>
-      <c r="B225" t="s">
-        <v>488</v>
       </c>
       <c r="C225">
         <v>772</v>
@@ -7240,15 +7240,15 @@
         <v>27</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A226" t="s">
+        <v>488</v>
+      </c>
+      <c r="B226" t="s">
         <v>489</v>
-      </c>
-      <c r="B226" t="s">
-        <v>490</v>
       </c>
       <c r="C226">
         <v>776</v>
@@ -7263,15 +7263,15 @@
         <v>27</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A227" t="s">
+        <v>490</v>
+      </c>
+      <c r="B227" t="s">
         <v>491</v>
-      </c>
-      <c r="B227" t="s">
-        <v>492</v>
       </c>
       <c r="C227">
         <v>780</v>
@@ -7286,15 +7286,15 @@
         <v>37</v>
       </c>
       <c r="G227" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A228" t="s">
+        <v>492</v>
+      </c>
+      <c r="B228" t="s">
         <v>493</v>
-      </c>
-      <c r="B228" t="s">
-        <v>494</v>
       </c>
       <c r="C228">
         <v>788</v>
@@ -7314,10 +7314,10 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A229" t="s">
+        <v>494</v>
+      </c>
+      <c r="B229" t="s">
         <v>495</v>
-      </c>
-      <c r="B229" t="s">
-        <v>496</v>
       </c>
       <c r="C229">
         <v>792</v>
@@ -7332,21 +7332,21 @@
         <v>11</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A230" t="s">
+        <v>496</v>
+      </c>
+      <c r="B230" t="s">
         <v>497</v>
-      </c>
-      <c r="B230" t="s">
-        <v>498</v>
       </c>
       <c r="C230">
         <v>795</v>
       </c>
       <c r="D230" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E230" t="s">
         <v>10</v>
@@ -7360,10 +7360,10 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A231" t="s">
+        <v>498</v>
+      </c>
+      <c r="B231" t="s">
         <v>499</v>
-      </c>
-      <c r="B231" t="s">
-        <v>500</v>
       </c>
       <c r="C231">
         <v>796</v>
@@ -7378,15 +7378,15 @@
         <v>37</v>
       </c>
       <c r="G231" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A232" t="s">
+        <v>500</v>
+      </c>
+      <c r="B232" t="s">
         <v>501</v>
-      </c>
-      <c r="B232" t="s">
-        <v>502</v>
       </c>
       <c r="C232">
         <v>798</v>
@@ -7401,15 +7401,15 @@
         <v>27</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A233" t="s">
+        <v>502</v>
+      </c>
+      <c r="B233" t="s">
         <v>503</v>
-      </c>
-      <c r="B233" t="s">
-        <v>504</v>
       </c>
       <c r="C233">
         <v>800</v>
@@ -7429,10 +7429,10 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A234" t="s">
+        <v>504</v>
+      </c>
+      <c r="B234" t="s">
         <v>505</v>
-      </c>
-      <c r="B234" t="s">
-        <v>506</v>
       </c>
       <c r="C234">
         <v>804</v>
@@ -7452,10 +7452,10 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A235" t="s">
+        <v>506</v>
+      </c>
+      <c r="B235" t="s">
         <v>507</v>
-      </c>
-      <c r="B235" t="s">
-        <v>508</v>
       </c>
       <c r="C235">
         <v>784</v>
@@ -7470,15 +7470,15 @@
         <v>11</v>
       </c>
       <c r="G235" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A236" t="s">
+        <v>508</v>
+      </c>
+      <c r="B236" t="s">
         <v>509</v>
-      </c>
-      <c r="B236" t="s">
-        <v>510</v>
       </c>
       <c r="C236">
         <v>826</v>
@@ -7498,10 +7498,10 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A237" t="s">
+        <v>510</v>
+      </c>
+      <c r="B237" t="s">
         <v>511</v>
-      </c>
-      <c r="B237" t="s">
-        <v>512</v>
       </c>
       <c r="C237">
         <v>834</v>
@@ -7521,10 +7521,10 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A238" t="s">
+        <v>512</v>
+      </c>
+      <c r="B238" t="s">
         <v>513</v>
-      </c>
-      <c r="B238" t="s">
-        <v>514</v>
       </c>
       <c r="C238">
         <v>581</v>
@@ -7539,15 +7539,15 @@
         <v>27</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A239" t="s">
+        <v>514</v>
+      </c>
+      <c r="B239" t="s">
         <v>515</v>
-      </c>
-      <c r="B239" t="s">
-        <v>516</v>
       </c>
       <c r="C239">
         <v>840</v>
@@ -7567,10 +7567,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A240" t="s">
+        <v>516</v>
+      </c>
+      <c r="B240" t="s">
         <v>517</v>
-      </c>
-      <c r="B240" t="s">
-        <v>518</v>
       </c>
       <c r="C240">
         <v>850</v>
@@ -7590,10 +7590,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A241" t="s">
+        <v>518</v>
+      </c>
+      <c r="B241" t="s">
         <v>519</v>
-      </c>
-      <c r="B241" t="s">
-        <v>520</v>
       </c>
       <c r="C241">
         <v>858</v>
@@ -7613,16 +7613,16 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A242" t="s">
+        <v>520</v>
+      </c>
+      <c r="B242" t="s">
         <v>521</v>
-      </c>
-      <c r="B242" t="s">
-        <v>522</v>
       </c>
       <c r="C242">
         <v>860</v>
       </c>
       <c r="D242" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E242" t="s">
         <v>10</v>
@@ -7636,10 +7636,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A243" t="s">
+        <v>522</v>
+      </c>
+      <c r="B243" t="s">
         <v>523</v>
-      </c>
-      <c r="B243" t="s">
-        <v>524</v>
       </c>
       <c r="C243">
         <v>548</v>
@@ -7654,15 +7654,15 @@
         <v>27</v>
       </c>
       <c r="G243" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A244" t="s">
+        <v>524</v>
+      </c>
+      <c r="B244" t="s">
         <v>525</v>
-      </c>
-      <c r="B244" t="s">
-        <v>526</v>
       </c>
       <c r="C244">
         <v>862</v>
@@ -7682,10 +7682,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A245" t="s">
+        <v>526</v>
+      </c>
+      <c r="B245" t="s">
         <v>527</v>
-      </c>
-      <c r="B245" t="s">
-        <v>528</v>
       </c>
       <c r="C245">
         <v>704</v>
@@ -7700,15 +7700,15 @@
         <v>11</v>
       </c>
       <c r="G245" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A246" t="s">
+        <v>528</v>
+      </c>
+      <c r="B246" t="s">
         <v>529</v>
-      </c>
-      <c r="B246" t="s">
-        <v>530</v>
       </c>
       <c r="C246">
         <v>876</v>
@@ -7723,15 +7723,15 @@
         <v>27</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A247" t="s">
+        <v>530</v>
+      </c>
+      <c r="B247" t="s">
         <v>531</v>
-      </c>
-      <c r="B247" t="s">
-        <v>532</v>
       </c>
       <c r="C247">
         <v>732</v>
@@ -7751,10 +7751,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A248" t="s">
+        <v>532</v>
+      </c>
+      <c r="B248" t="s">
         <v>533</v>
-      </c>
-      <c r="B248" t="s">
-        <v>534</v>
       </c>
       <c r="C248">
         <v>887</v>
@@ -7769,15 +7769,15 @@
         <v>11</v>
       </c>
       <c r="G248" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A249" t="s">
+        <v>534</v>
+      </c>
+      <c r="B249" t="s">
         <v>535</v>
-      </c>
-      <c r="B249" t="s">
-        <v>536</v>
       </c>
       <c r="C249">
         <v>894</v>
@@ -7797,10 +7797,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A250" t="s">
+        <v>536</v>
+      </c>
+      <c r="B250" t="s">
         <v>537</v>
-      </c>
-      <c r="B250" t="s">
-        <v>538</v>
       </c>
       <c r="C250">
         <v>716</v>
@@ -7825,8 +7825,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94796c5baa2ef88ac6145701948dc8f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e880ceb9264c792c54763cc60e020778" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -7839,6 +7854,14 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7857,6 +7880,50 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7989,23 +8056,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68005736-06FA-4D64-8A47-A5C2FE90D8F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE6E345-17DA-4015-8573-D37D65FCD6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8974A86F-D576-4CE7-A871-E52C0BC6C628}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DC56ECA-7BAF-47C0-907D-58E53A0DB938}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -8021,21 +8090,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68005736-06FA-4D64-8A47-A5C2FE90D8F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE6E345-17DA-4015-8573-D37D65FCD6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed error in middle east string
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Country Reference.xlsx
+++ b/mppsteel/data/import_data/Country Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB39D86-AA5D-46B1-9DA8-FA665A72CE5A}"/>
+  <xr:revisionPtr revIDLastSave="559" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26749FE-B778-4FCF-98E3-18214BDA9046}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{399614B1-7431-4F70-9F99-85E1D48DE75C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="545">
   <si>
     <t>Country</t>
   </si>
@@ -868,9 +868,6 @@
   </si>
   <si>
     <t>JOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle East </t>
   </si>
   <si>
     <t>Kazakhstan</t>
@@ -2054,7 +2051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2203,7 +2200,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -2295,7 +2292,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -2410,7 +2407,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -2525,7 +2522,7 @@
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
@@ -2686,12 +2683,12 @@
         <v>11</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B28" t="s">
         <v>86</v>
@@ -2893,7 +2890,7 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
@@ -3008,7 +3005,7 @@
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
@@ -3238,7 +3235,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
@@ -3261,7 +3258,7 @@
         <v>27</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
@@ -3353,7 +3350,7 @@
         <v>27</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.5">
@@ -3537,7 +3534,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.5">
@@ -3841,7 +3838,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B78" t="s">
         <v>191</v>
@@ -3905,7 +3902,7 @@
         <v>27</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.5">
@@ -3997,7 +3994,7 @@
         <v>27</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.5">
@@ -4020,7 +4017,7 @@
         <v>23</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.5">
@@ -4089,7 +4086,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.5">
@@ -4204,7 +4201,7 @@
         <v>37</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.5">
@@ -4273,7 +4270,7 @@
         <v>27</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.5">
@@ -4434,7 +4431,7 @@
         <v>27</v>
       </c>
       <c r="G103" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.5">
@@ -4572,7 +4569,7 @@
         <v>11</v>
       </c>
       <c r="G109" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.5">
@@ -4687,7 +4684,7 @@
         <v>11</v>
       </c>
       <c r="G114" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.5">
@@ -4756,7 +4753,7 @@
         <v>271</v>
       </c>
       <c r="G117" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.5">
@@ -4802,21 +4799,21 @@
         <v>11</v>
       </c>
       <c r="G119" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
+        <v>277</v>
+      </c>
+      <c r="B120" t="s">
         <v>278</v>
-      </c>
-      <c r="B120" t="s">
-        <v>279</v>
       </c>
       <c r="C120">
         <v>398</v>
       </c>
       <c r="D120" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E120" t="s">
         <v>10</v>
@@ -4830,10 +4827,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
+        <v>280</v>
+      </c>
+      <c r="B121" t="s">
         <v>281</v>
-      </c>
-      <c r="B121" t="s">
-        <v>282</v>
       </c>
       <c r="C121">
         <v>404</v>
@@ -4853,10 +4850,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
+        <v>282</v>
+      </c>
+      <c r="B122" t="s">
         <v>283</v>
-      </c>
-      <c r="B122" t="s">
-        <v>284</v>
       </c>
       <c r="C122">
         <v>296</v>
@@ -4871,15 +4868,15 @@
         <v>27</v>
       </c>
       <c r="G122" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
+        <v>284</v>
+      </c>
+      <c r="B123" t="s">
         <v>285</v>
-      </c>
-      <c r="B123" t="s">
-        <v>286</v>
       </c>
       <c r="C123">
         <v>414</v>
@@ -4899,16 +4896,16 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
+        <v>286</v>
+      </c>
+      <c r="B124" t="s">
         <v>287</v>
-      </c>
-      <c r="B124" t="s">
-        <v>288</v>
       </c>
       <c r="C124">
         <v>417</v>
       </c>
       <c r="D124" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -4922,10 +4919,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
+        <v>288</v>
+      </c>
+      <c r="B125" t="s">
         <v>289</v>
-      </c>
-      <c r="B125" t="s">
-        <v>290</v>
       </c>
       <c r="C125">
         <v>418</v>
@@ -4940,15 +4937,15 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
+        <v>290</v>
+      </c>
+      <c r="B126" t="s">
         <v>291</v>
-      </c>
-      <c r="B126" t="s">
-        <v>292</v>
       </c>
       <c r="C126">
         <v>428</v>
@@ -4968,10 +4965,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
+        <v>292</v>
+      </c>
+      <c r="B127" t="s">
         <v>293</v>
-      </c>
-      <c r="B127" t="s">
-        <v>294</v>
       </c>
       <c r="C127">
         <v>422</v>
@@ -4991,10 +4988,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
+        <v>294</v>
+      </c>
+      <c r="B128" t="s">
         <v>295</v>
-      </c>
-      <c r="B128" t="s">
-        <v>296</v>
       </c>
       <c r="C128">
         <v>426</v>
@@ -5014,10 +5011,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A129" t="s">
+        <v>296</v>
+      </c>
+      <c r="B129" t="s">
         <v>297</v>
-      </c>
-      <c r="B129" t="s">
-        <v>298</v>
       </c>
       <c r="C129">
         <v>430</v>
@@ -5037,10 +5034,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
+        <v>298</v>
+      </c>
+      <c r="B130" t="s">
         <v>299</v>
-      </c>
-      <c r="B130" t="s">
-        <v>300</v>
       </c>
       <c r="C130">
         <v>434</v>
@@ -5060,10 +5057,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A131" t="s">
+        <v>300</v>
+      </c>
+      <c r="B131" t="s">
         <v>301</v>
-      </c>
-      <c r="B131" t="s">
-        <v>302</v>
       </c>
       <c r="C131">
         <v>438</v>
@@ -5083,10 +5080,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A132" t="s">
+        <v>302</v>
+      </c>
+      <c r="B132" t="s">
         <v>303</v>
-      </c>
-      <c r="B132" t="s">
-        <v>304</v>
       </c>
       <c r="C132">
         <v>440</v>
@@ -5106,10 +5103,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A133" t="s">
+        <v>304</v>
+      </c>
+      <c r="B133" t="s">
         <v>305</v>
-      </c>
-      <c r="B133" t="s">
-        <v>306</v>
       </c>
       <c r="C133">
         <v>442</v>
@@ -5129,10 +5126,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
+        <v>306</v>
+      </c>
+      <c r="B134" t="s">
         <v>307</v>
-      </c>
-      <c r="B134" t="s">
-        <v>308</v>
       </c>
       <c r="C134">
         <v>450</v>
@@ -5152,10 +5149,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A135" t="s">
+        <v>308</v>
+      </c>
+      <c r="B135" t="s">
         <v>309</v>
-      </c>
-      <c r="B135" t="s">
-        <v>310</v>
       </c>
       <c r="C135">
         <v>454</v>
@@ -5175,10 +5172,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A136" t="s">
+        <v>310</v>
+      </c>
+      <c r="B136" t="s">
         <v>311</v>
-      </c>
-      <c r="B136" t="s">
-        <v>312</v>
       </c>
       <c r="C136">
         <v>458</v>
@@ -5193,15 +5190,15 @@
         <v>11</v>
       </c>
       <c r="G136" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A137" t="s">
+        <v>312</v>
+      </c>
+      <c r="B137" t="s">
         <v>313</v>
-      </c>
-      <c r="B137" t="s">
-        <v>314</v>
       </c>
       <c r="C137">
         <v>462</v>
@@ -5216,15 +5213,15 @@
         <v>11</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
+        <v>314</v>
+      </c>
+      <c r="B138" t="s">
         <v>315</v>
-      </c>
-      <c r="B138" t="s">
-        <v>316</v>
       </c>
       <c r="C138">
         <v>466</v>
@@ -5244,10 +5241,10 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A139" t="s">
+        <v>316</v>
+      </c>
+      <c r="B139" t="s">
         <v>317</v>
-      </c>
-      <c r="B139" t="s">
-        <v>318</v>
       </c>
       <c r="C139">
         <v>470</v>
@@ -5267,10 +5264,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A140" t="s">
+        <v>318</v>
+      </c>
+      <c r="B140" t="s">
         <v>319</v>
-      </c>
-      <c r="B140" t="s">
-        <v>320</v>
       </c>
       <c r="C140">
         <v>584</v>
@@ -5285,15 +5282,15 @@
         <v>27</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A141" t="s">
+        <v>320</v>
+      </c>
+      <c r="B141" t="s">
         <v>321</v>
-      </c>
-      <c r="B141" t="s">
-        <v>322</v>
       </c>
       <c r="C141">
         <v>474</v>
@@ -5313,10 +5310,10 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A142" t="s">
+        <v>322</v>
+      </c>
+      <c r="B142" t="s">
         <v>323</v>
-      </c>
-      <c r="B142" t="s">
-        <v>324</v>
       </c>
       <c r="C142">
         <v>478</v>
@@ -5336,10 +5333,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A143" t="s">
+        <v>324</v>
+      </c>
+      <c r="B143" t="s">
         <v>325</v>
-      </c>
-      <c r="B143" t="s">
-        <v>326</v>
       </c>
       <c r="C143">
         <v>480</v>
@@ -5359,10 +5356,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A144" t="s">
+        <v>326</v>
+      </c>
+      <c r="B144" t="s">
         <v>327</v>
-      </c>
-      <c r="B144" t="s">
-        <v>328</v>
       </c>
       <c r="C144">
         <v>175</v>
@@ -5382,10 +5379,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A145" t="s">
+        <v>328</v>
+      </c>
+      <c r="B145" t="s">
         <v>329</v>
-      </c>
-      <c r="B145" t="s">
-        <v>330</v>
       </c>
       <c r="C145">
         <v>484</v>
@@ -5405,10 +5402,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A146" t="s">
+        <v>330</v>
+      </c>
+      <c r="B146" t="s">
         <v>331</v>
-      </c>
-      <c r="B146" t="s">
-        <v>332</v>
       </c>
       <c r="C146">
         <v>583</v>
@@ -5423,15 +5420,15 @@
         <v>27</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A147" t="s">
+        <v>332</v>
+      </c>
+      <c r="B147" t="s">
         <v>333</v>
-      </c>
-      <c r="B147" t="s">
-        <v>334</v>
       </c>
       <c r="C147">
         <v>492</v>
@@ -5451,10 +5448,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A148" t="s">
+        <v>334</v>
+      </c>
+      <c r="B148" t="s">
         <v>335</v>
-      </c>
-      <c r="B148" t="s">
-        <v>336</v>
       </c>
       <c r="C148">
         <v>496</v>
@@ -5469,15 +5466,15 @@
         <v>11</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A149" t="s">
+        <v>336</v>
+      </c>
+      <c r="B149" t="s">
         <v>337</v>
-      </c>
-      <c r="B149" t="s">
-        <v>338</v>
       </c>
       <c r="C149">
         <v>499</v>
@@ -5497,10 +5494,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A150" t="s">
+        <v>338</v>
+      </c>
+      <c r="B150" t="s">
         <v>339</v>
-      </c>
-      <c r="B150" t="s">
-        <v>340</v>
       </c>
       <c r="C150">
         <v>500</v>
@@ -5520,10 +5517,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A151" t="s">
+        <v>340</v>
+      </c>
+      <c r="B151" t="s">
         <v>341</v>
-      </c>
-      <c r="B151" t="s">
-        <v>342</v>
       </c>
       <c r="C151">
         <v>504</v>
@@ -5543,10 +5540,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A152" t="s">
+        <v>342</v>
+      </c>
+      <c r="B152" t="s">
         <v>343</v>
-      </c>
-      <c r="B152" t="s">
-        <v>344</v>
       </c>
       <c r="C152">
         <v>508</v>
@@ -5566,10 +5563,10 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A153" t="s">
+        <v>344</v>
+      </c>
+      <c r="B153" t="s">
         <v>345</v>
-      </c>
-      <c r="B153" t="s">
-        <v>346</v>
       </c>
       <c r="C153">
         <v>104</v>
@@ -5584,15 +5581,15 @@
         <v>11</v>
       </c>
       <c r="G153" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A154" t="s">
+        <v>346</v>
+      </c>
+      <c r="B154" t="s">
         <v>347</v>
-      </c>
-      <c r="B154" t="s">
-        <v>348</v>
       </c>
       <c r="C154">
         <v>516</v>
@@ -5612,10 +5609,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A155" t="s">
+        <v>348</v>
+      </c>
+      <c r="B155" t="s">
         <v>349</v>
-      </c>
-      <c r="B155" t="s">
-        <v>350</v>
       </c>
       <c r="C155">
         <v>520</v>
@@ -5630,15 +5627,15 @@
         <v>27</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A156" t="s">
+        <v>350</v>
+      </c>
+      <c r="B156" t="s">
         <v>351</v>
-      </c>
-      <c r="B156" t="s">
-        <v>352</v>
       </c>
       <c r="C156">
         <v>524</v>
@@ -5653,15 +5650,15 @@
         <v>11</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A157" t="s">
+        <v>352</v>
+      </c>
+      <c r="B157" t="s">
         <v>353</v>
-      </c>
-      <c r="B157" t="s">
-        <v>354</v>
       </c>
       <c r="C157">
         <v>528</v>
@@ -5681,10 +5678,10 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A158" t="s">
+        <v>354</v>
+      </c>
+      <c r="B158" t="s">
         <v>355</v>
-      </c>
-      <c r="B158" t="s">
-        <v>356</v>
       </c>
       <c r="C158">
         <v>540</v>
@@ -5699,15 +5696,15 @@
         <v>27</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A159" t="s">
+        <v>356</v>
+      </c>
+      <c r="B159" t="s">
         <v>357</v>
-      </c>
-      <c r="B159" t="s">
-        <v>358</v>
       </c>
       <c r="C159">
         <v>554</v>
@@ -5722,15 +5719,15 @@
         <v>27</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A160" t="s">
+        <v>358</v>
+      </c>
+      <c r="B160" t="s">
         <v>359</v>
-      </c>
-      <c r="B160" t="s">
-        <v>360</v>
       </c>
       <c r="C160">
         <v>558</v>
@@ -5750,10 +5747,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A161" t="s">
+        <v>360</v>
+      </c>
+      <c r="B161" t="s">
         <v>361</v>
-      </c>
-      <c r="B161" t="s">
-        <v>362</v>
       </c>
       <c r="C161">
         <v>562</v>
@@ -5773,10 +5770,10 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A162" t="s">
+        <v>362</v>
+      </c>
+      <c r="B162" t="s">
         <v>363</v>
-      </c>
-      <c r="B162" t="s">
-        <v>364</v>
       </c>
       <c r="C162">
         <v>566</v>
@@ -5796,10 +5793,10 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A163" t="s">
+        <v>364</v>
+      </c>
+      <c r="B163" t="s">
         <v>365</v>
-      </c>
-      <c r="B163" t="s">
-        <v>366</v>
       </c>
       <c r="C163">
         <v>570</v>
@@ -5814,15 +5811,15 @@
         <v>27</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A164" t="s">
+        <v>366</v>
+      </c>
+      <c r="B164" t="s">
         <v>367</v>
-      </c>
-      <c r="B164" t="s">
-        <v>368</v>
       </c>
       <c r="C164">
         <v>574</v>
@@ -5837,15 +5834,15 @@
         <v>27</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A165" t="s">
+        <v>368</v>
+      </c>
+      <c r="B165" t="s">
         <v>369</v>
-      </c>
-      <c r="B165" t="s">
-        <v>370</v>
       </c>
       <c r="C165">
         <v>807</v>
@@ -5865,10 +5862,10 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A166" t="s">
+        <v>370</v>
+      </c>
+      <c r="B166" t="s">
         <v>371</v>
-      </c>
-      <c r="B166" t="s">
-        <v>372</v>
       </c>
       <c r="C166">
         <v>580</v>
@@ -5883,15 +5880,15 @@
         <v>27</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A167" t="s">
+        <v>372</v>
+      </c>
+      <c r="B167" t="s">
         <v>373</v>
-      </c>
-      <c r="B167" t="s">
-        <v>374</v>
       </c>
       <c r="C167">
         <v>578</v>
@@ -5911,10 +5908,10 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A168" t="s">
+        <v>374</v>
+      </c>
+      <c r="B168" t="s">
         <v>375</v>
-      </c>
-      <c r="B168" t="s">
-        <v>376</v>
       </c>
       <c r="C168">
         <v>512</v>
@@ -5934,10 +5931,10 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A169" t="s">
+        <v>376</v>
+      </c>
+      <c r="B169" t="s">
         <v>377</v>
-      </c>
-      <c r="B169" t="s">
-        <v>378</v>
       </c>
       <c r="C169">
         <v>586</v>
@@ -5952,15 +5949,15 @@
         <v>11</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A170" t="s">
+        <v>378</v>
+      </c>
+      <c r="B170" t="s">
         <v>379</v>
-      </c>
-      <c r="B170" t="s">
-        <v>380</v>
       </c>
       <c r="C170">
         <v>585</v>
@@ -5975,15 +5972,15 @@
         <v>27</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A171" t="s">
+        <v>380</v>
+      </c>
+      <c r="B171" t="s">
         <v>381</v>
-      </c>
-      <c r="B171" t="s">
-        <v>382</v>
       </c>
       <c r="C171">
         <v>591</v>
@@ -6003,10 +6000,10 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A172" t="s">
+        <v>382</v>
+      </c>
+      <c r="B172" t="s">
         <v>383</v>
-      </c>
-      <c r="B172" t="s">
-        <v>384</v>
       </c>
       <c r="C172">
         <v>598</v>
@@ -6021,15 +6018,15 @@
         <v>27</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A173" t="s">
+        <v>384</v>
+      </c>
+      <c r="B173" t="s">
         <v>385</v>
-      </c>
-      <c r="B173" t="s">
-        <v>386</v>
       </c>
       <c r="C173">
         <v>600</v>
@@ -6049,10 +6046,10 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A174" t="s">
+        <v>386</v>
+      </c>
+      <c r="B174" t="s">
         <v>387</v>
-      </c>
-      <c r="B174" t="s">
-        <v>388</v>
       </c>
       <c r="C174">
         <v>604</v>
@@ -6072,10 +6069,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A175" t="s">
+        <v>388</v>
+      </c>
+      <c r="B175" t="s">
         <v>389</v>
-      </c>
-      <c r="B175" t="s">
-        <v>390</v>
       </c>
       <c r="C175">
         <v>608</v>
@@ -6090,15 +6087,15 @@
         <v>11</v>
       </c>
       <c r="G175" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A176" t="s">
+        <v>390</v>
+      </c>
+      <c r="B176" t="s">
         <v>391</v>
-      </c>
-      <c r="B176" t="s">
-        <v>392</v>
       </c>
       <c r="C176">
         <v>612</v>
@@ -6113,15 +6110,15 @@
         <v>27</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A177" t="s">
+        <v>392</v>
+      </c>
+      <c r="B177" t="s">
         <v>393</v>
-      </c>
-      <c r="B177" t="s">
-        <v>394</v>
       </c>
       <c r="C177">
         <v>616</v>
@@ -6141,10 +6138,10 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A178" t="s">
+        <v>394</v>
+      </c>
+      <c r="B178" t="s">
         <v>395</v>
-      </c>
-      <c r="B178" t="s">
-        <v>396</v>
       </c>
       <c r="C178">
         <v>620</v>
@@ -6164,10 +6161,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A179" t="s">
+        <v>396</v>
+      </c>
+      <c r="B179" t="s">
         <v>397</v>
-      </c>
-      <c r="B179" t="s">
-        <v>398</v>
       </c>
       <c r="C179">
         <v>630</v>
@@ -6187,10 +6184,10 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A180" t="s">
+        <v>398</v>
+      </c>
+      <c r="B180" t="s">
         <v>399</v>
-      </c>
-      <c r="B180" t="s">
-        <v>400</v>
       </c>
       <c r="C180">
         <v>634</v>
@@ -6210,10 +6207,10 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A181" t="s">
+        <v>400</v>
+      </c>
+      <c r="B181" t="s">
         <v>401</v>
-      </c>
-      <c r="B181" t="s">
-        <v>402</v>
       </c>
       <c r="C181">
         <v>410</v>
@@ -6228,15 +6225,15 @@
         <v>11</v>
       </c>
       <c r="G181" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A182" t="s">
+        <v>402</v>
+      </c>
+      <c r="B182" t="s">
         <v>403</v>
-      </c>
-      <c r="B182" t="s">
-        <v>404</v>
       </c>
       <c r="C182">
         <v>498</v>
@@ -6256,10 +6253,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A183" t="s">
+        <v>404</v>
+      </c>
+      <c r="B183" t="s">
         <v>405</v>
-      </c>
-      <c r="B183" t="s">
-        <v>406</v>
       </c>
       <c r="C183">
         <v>638</v>
@@ -6279,10 +6276,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A184" t="s">
+        <v>406</v>
+      </c>
+      <c r="B184" t="s">
         <v>407</v>
-      </c>
-      <c r="B184" t="s">
-        <v>408</v>
       </c>
       <c r="C184">
         <v>642</v>
@@ -6302,10 +6299,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A185" t="s">
+        <v>408</v>
+      </c>
+      <c r="B185" t="s">
         <v>409</v>
-      </c>
-      <c r="B185" t="s">
-        <v>410</v>
       </c>
       <c r="C185">
         <v>643</v>
@@ -6325,10 +6322,10 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A186" t="s">
+        <v>410</v>
+      </c>
+      <c r="B186" t="s">
         <v>411</v>
-      </c>
-      <c r="B186" t="s">
-        <v>412</v>
       </c>
       <c r="C186">
         <v>646</v>
@@ -6348,10 +6345,10 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A187" t="s">
+        <v>412</v>
+      </c>
+      <c r="B187" t="s">
         <v>413</v>
-      </c>
-      <c r="B187" t="s">
-        <v>414</v>
       </c>
       <c r="C187">
         <v>652</v>
@@ -6371,10 +6368,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A188" t="s">
+        <v>414</v>
+      </c>
+      <c r="B188" t="s">
         <v>415</v>
-      </c>
-      <c r="B188" t="s">
-        <v>416</v>
       </c>
       <c r="C188">
         <v>654</v>
@@ -6389,15 +6386,15 @@
         <v>23</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A189" t="s">
+        <v>416</v>
+      </c>
+      <c r="B189" t="s">
         <v>417</v>
-      </c>
-      <c r="B189" t="s">
-        <v>418</v>
       </c>
       <c r="C189">
         <v>659</v>
@@ -6417,10 +6414,10 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A190" t="s">
+        <v>418</v>
+      </c>
+      <c r="B190" t="s">
         <v>419</v>
-      </c>
-      <c r="B190" t="s">
-        <v>420</v>
       </c>
       <c r="C190">
         <v>662</v>
@@ -6440,10 +6437,10 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A191" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B191" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C191">
         <v>663</v>
@@ -6463,10 +6460,10 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A192" t="s">
+        <v>421</v>
+      </c>
+      <c r="B192" t="s">
         <v>422</v>
-      </c>
-      <c r="B192" t="s">
-        <v>423</v>
       </c>
       <c r="C192">
         <v>666</v>
@@ -6486,10 +6483,10 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A193" t="s">
+        <v>423</v>
+      </c>
+      <c r="B193" t="s">
         <v>424</v>
-      </c>
-      <c r="B193" t="s">
-        <v>425</v>
       </c>
       <c r="C193">
         <v>670</v>
@@ -6509,10 +6506,10 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A194" t="s">
+        <v>425</v>
+      </c>
+      <c r="B194" t="s">
         <v>426</v>
-      </c>
-      <c r="B194" t="s">
-        <v>427</v>
       </c>
       <c r="C194">
         <v>882</v>
@@ -6527,15 +6524,15 @@
         <v>27</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A195" t="s">
+        <v>427</v>
+      </c>
+      <c r="B195" t="s">
         <v>428</v>
-      </c>
-      <c r="B195" t="s">
-        <v>429</v>
       </c>
       <c r="C195">
         <v>674</v>
@@ -6555,10 +6552,10 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A196" t="s">
+        <v>429</v>
+      </c>
+      <c r="B196" t="s">
         <v>430</v>
-      </c>
-      <c r="B196" t="s">
-        <v>431</v>
       </c>
       <c r="C196">
         <v>678</v>
@@ -6578,10 +6575,10 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A197" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B197" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C197">
         <v>680</v>
@@ -6601,10 +6598,10 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A198" t="s">
+        <v>432</v>
+      </c>
+      <c r="B198" t="s">
         <v>433</v>
-      </c>
-      <c r="B198" t="s">
-        <v>434</v>
       </c>
       <c r="C198">
         <v>682</v>
@@ -6624,10 +6621,10 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A199" t="s">
+        <v>434</v>
+      </c>
+      <c r="B199" t="s">
         <v>435</v>
-      </c>
-      <c r="B199" t="s">
-        <v>436</v>
       </c>
       <c r="C199">
         <v>686</v>
@@ -6647,10 +6644,10 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A200" t="s">
+        <v>436</v>
+      </c>
+      <c r="B200" t="s">
         <v>437</v>
-      </c>
-      <c r="B200" t="s">
-        <v>438</v>
       </c>
       <c r="C200">
         <v>688</v>
@@ -6670,10 +6667,10 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A201" t="s">
+        <v>438</v>
+      </c>
+      <c r="B201" t="s">
         <v>439</v>
-      </c>
-      <c r="B201" t="s">
-        <v>440</v>
       </c>
       <c r="C201">
         <v>690</v>
@@ -6688,15 +6685,15 @@
         <v>23</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A202" t="s">
+        <v>440</v>
+      </c>
+      <c r="B202" t="s">
         <v>441</v>
-      </c>
-      <c r="B202" t="s">
-        <v>442</v>
       </c>
       <c r="C202">
         <v>694</v>
@@ -6716,10 +6713,10 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A203" t="s">
+        <v>442</v>
+      </c>
+      <c r="B203" t="s">
         <v>443</v>
-      </c>
-      <c r="B203" t="s">
-        <v>444</v>
       </c>
       <c r="C203">
         <v>702</v>
@@ -6734,15 +6731,15 @@
         <v>11</v>
       </c>
       <c r="G203" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A204" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B204" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C204">
         <v>534</v>
@@ -6757,15 +6754,15 @@
         <v>37</v>
       </c>
       <c r="G204" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A205" t="s">
+        <v>445</v>
+      </c>
+      <c r="B205" t="s">
         <v>446</v>
-      </c>
-      <c r="B205" t="s">
-        <v>447</v>
       </c>
       <c r="C205">
         <v>703</v>
@@ -6785,10 +6782,10 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A206" t="s">
+        <v>447</v>
+      </c>
+      <c r="B206" t="s">
         <v>448</v>
-      </c>
-      <c r="B206" t="s">
-        <v>449</v>
       </c>
       <c r="C206">
         <v>705</v>
@@ -6808,10 +6805,10 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A207" t="s">
+        <v>449</v>
+      </c>
+      <c r="B207" t="s">
         <v>450</v>
-      </c>
-      <c r="B207" t="s">
-        <v>451</v>
       </c>
       <c r="C207">
         <v>90</v>
@@ -6826,15 +6823,15 @@
         <v>27</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A208" t="s">
+        <v>451</v>
+      </c>
+      <c r="B208" t="s">
         <v>452</v>
-      </c>
-      <c r="B208" t="s">
-        <v>453</v>
       </c>
       <c r="C208">
         <v>706</v>
@@ -6854,10 +6851,10 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A209" t="s">
+        <v>453</v>
+      </c>
+      <c r="B209" t="s">
         <v>454</v>
-      </c>
-      <c r="B209" t="s">
-        <v>455</v>
       </c>
       <c r="C209">
         <v>710</v>
@@ -6877,10 +6874,10 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A210" t="s">
+        <v>455</v>
+      </c>
+      <c r="B210" t="s">
         <v>456</v>
-      </c>
-      <c r="B210" t="s">
-        <v>457</v>
       </c>
       <c r="C210">
         <v>239</v>
@@ -6900,10 +6897,10 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A211" t="s">
+        <v>457</v>
+      </c>
+      <c r="B211" t="s">
         <v>458</v>
-      </c>
-      <c r="B211" t="s">
-        <v>459</v>
       </c>
       <c r="C211">
         <v>728</v>
@@ -6923,10 +6920,10 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A212" t="s">
+        <v>459</v>
+      </c>
+      <c r="B212" t="s">
         <v>460</v>
-      </c>
-      <c r="B212" t="s">
-        <v>461</v>
       </c>
       <c r="C212">
         <v>724</v>
@@ -6946,10 +6943,10 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A213" t="s">
+        <v>461</v>
+      </c>
+      <c r="B213" t="s">
         <v>462</v>
-      </c>
-      <c r="B213" t="s">
-        <v>463</v>
       </c>
       <c r="C213">
         <v>144</v>
@@ -6964,15 +6961,15 @@
         <v>11</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A214" t="s">
+        <v>463</v>
+      </c>
+      <c r="B214" t="s">
         <v>464</v>
-      </c>
-      <c r="B214" t="s">
-        <v>465</v>
       </c>
       <c r="C214">
         <v>275</v>
@@ -6992,10 +6989,10 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A215" t="s">
+        <v>465</v>
+      </c>
+      <c r="B215" t="s">
         <v>466</v>
-      </c>
-      <c r="B215" t="s">
-        <v>467</v>
       </c>
       <c r="C215">
         <v>729</v>
@@ -7015,10 +7012,10 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A216" t="s">
+        <v>467</v>
+      </c>
+      <c r="B216" t="s">
         <v>468</v>
-      </c>
-      <c r="B216" t="s">
-        <v>469</v>
       </c>
       <c r="C216">
         <v>740</v>
@@ -7038,10 +7035,10 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A217" t="s">
+        <v>469</v>
+      </c>
+      <c r="B217" t="s">
         <v>470</v>
-      </c>
-      <c r="B217" t="s">
-        <v>471</v>
       </c>
       <c r="C217">
         <v>744</v>
@@ -7061,10 +7058,10 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A218" t="s">
+        <v>471</v>
+      </c>
+      <c r="B218" t="s">
         <v>472</v>
-      </c>
-      <c r="B218" t="s">
-        <v>473</v>
       </c>
       <c r="C218">
         <v>752</v>
@@ -7084,10 +7081,10 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A219" t="s">
+        <v>473</v>
+      </c>
+      <c r="B219" t="s">
         <v>474</v>
-      </c>
-      <c r="B219" t="s">
-        <v>475</v>
       </c>
       <c r="C219">
         <v>756</v>
@@ -7107,10 +7104,10 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A220" t="s">
+        <v>475</v>
+      </c>
+      <c r="B220" t="s">
         <v>476</v>
-      </c>
-      <c r="B220" t="s">
-        <v>477</v>
       </c>
       <c r="C220">
         <v>760</v>
@@ -7130,16 +7127,16 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A221" t="s">
+        <v>477</v>
+      </c>
+      <c r="B221" t="s">
         <v>478</v>
-      </c>
-      <c r="B221" t="s">
-        <v>479</v>
       </c>
       <c r="C221">
         <v>762</v>
       </c>
       <c r="D221" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E221" t="s">
         <v>10</v>
@@ -7153,10 +7150,10 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A222" t="s">
+        <v>479</v>
+      </c>
+      <c r="B222" t="s">
         <v>480</v>
-      </c>
-      <c r="B222" t="s">
-        <v>481</v>
       </c>
       <c r="C222">
         <v>764</v>
@@ -7171,15 +7168,15 @@
         <v>11</v>
       </c>
       <c r="G222" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A223" t="s">
+        <v>481</v>
+      </c>
+      <c r="B223" t="s">
         <v>482</v>
-      </c>
-      <c r="B223" t="s">
-        <v>483</v>
       </c>
       <c r="C223">
         <v>626</v>
@@ -7194,15 +7191,15 @@
         <v>11</v>
       </c>
       <c r="G223" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A224" t="s">
+        <v>483</v>
+      </c>
+      <c r="B224" t="s">
         <v>484</v>
-      </c>
-      <c r="B224" t="s">
-        <v>485</v>
       </c>
       <c r="C224">
         <v>768</v>
@@ -7222,10 +7219,10 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A225" t="s">
+        <v>485</v>
+      </c>
+      <c r="B225" t="s">
         <v>486</v>
-      </c>
-      <c r="B225" t="s">
-        <v>487</v>
       </c>
       <c r="C225">
         <v>772</v>
@@ -7240,15 +7237,15 @@
         <v>27</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A226" t="s">
+        <v>487</v>
+      </c>
+      <c r="B226" t="s">
         <v>488</v>
-      </c>
-      <c r="B226" t="s">
-        <v>489</v>
       </c>
       <c r="C226">
         <v>776</v>
@@ -7263,15 +7260,15 @@
         <v>27</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A227" t="s">
+        <v>489</v>
+      </c>
+      <c r="B227" t="s">
         <v>490</v>
-      </c>
-      <c r="B227" t="s">
-        <v>491</v>
       </c>
       <c r="C227">
         <v>780</v>
@@ -7286,15 +7283,15 @@
         <v>37</v>
       </c>
       <c r="G227" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A228" t="s">
+        <v>491</v>
+      </c>
+      <c r="B228" t="s">
         <v>492</v>
-      </c>
-      <c r="B228" t="s">
-        <v>493</v>
       </c>
       <c r="C228">
         <v>788</v>
@@ -7314,10 +7311,10 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A229" t="s">
+        <v>493</v>
+      </c>
+      <c r="B229" t="s">
         <v>494</v>
-      </c>
-      <c r="B229" t="s">
-        <v>495</v>
       </c>
       <c r="C229">
         <v>792</v>
@@ -7332,21 +7329,21 @@
         <v>11</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A230" t="s">
+        <v>495</v>
+      </c>
+      <c r="B230" t="s">
         <v>496</v>
-      </c>
-      <c r="B230" t="s">
-        <v>497</v>
       </c>
       <c r="C230">
         <v>795</v>
       </c>
       <c r="D230" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E230" t="s">
         <v>10</v>
@@ -7360,10 +7357,10 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A231" t="s">
+        <v>497</v>
+      </c>
+      <c r="B231" t="s">
         <v>498</v>
-      </c>
-      <c r="B231" t="s">
-        <v>499</v>
       </c>
       <c r="C231">
         <v>796</v>
@@ -7378,15 +7375,15 @@
         <v>37</v>
       </c>
       <c r="G231" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A232" t="s">
+        <v>499</v>
+      </c>
+      <c r="B232" t="s">
         <v>500</v>
-      </c>
-      <c r="B232" t="s">
-        <v>501</v>
       </c>
       <c r="C232">
         <v>798</v>
@@ -7401,15 +7398,15 @@
         <v>27</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A233" t="s">
+        <v>501</v>
+      </c>
+      <c r="B233" t="s">
         <v>502</v>
-      </c>
-      <c r="B233" t="s">
-        <v>503</v>
       </c>
       <c r="C233">
         <v>800</v>
@@ -7429,10 +7426,10 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A234" t="s">
+        <v>503</v>
+      </c>
+      <c r="B234" t="s">
         <v>504</v>
-      </c>
-      <c r="B234" t="s">
-        <v>505</v>
       </c>
       <c r="C234">
         <v>804</v>
@@ -7452,10 +7449,10 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A235" t="s">
+        <v>505</v>
+      </c>
+      <c r="B235" t="s">
         <v>506</v>
-      </c>
-      <c r="B235" t="s">
-        <v>507</v>
       </c>
       <c r="C235">
         <v>784</v>
@@ -7470,15 +7467,15 @@
         <v>11</v>
       </c>
       <c r="G235" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A236" t="s">
+        <v>507</v>
+      </c>
+      <c r="B236" t="s">
         <v>508</v>
-      </c>
-      <c r="B236" t="s">
-        <v>509</v>
       </c>
       <c r="C236">
         <v>826</v>
@@ -7498,10 +7495,10 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A237" t="s">
+        <v>509</v>
+      </c>
+      <c r="B237" t="s">
         <v>510</v>
-      </c>
-      <c r="B237" t="s">
-        <v>511</v>
       </c>
       <c r="C237">
         <v>834</v>
@@ -7521,10 +7518,10 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A238" t="s">
+        <v>511</v>
+      </c>
+      <c r="B238" t="s">
         <v>512</v>
-      </c>
-      <c r="B238" t="s">
-        <v>513</v>
       </c>
       <c r="C238">
         <v>581</v>
@@ -7539,15 +7536,15 @@
         <v>27</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A239" t="s">
+        <v>513</v>
+      </c>
+      <c r="B239" t="s">
         <v>514</v>
-      </c>
-      <c r="B239" t="s">
-        <v>515</v>
       </c>
       <c r="C239">
         <v>840</v>
@@ -7567,10 +7564,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A240" t="s">
+        <v>515</v>
+      </c>
+      <c r="B240" t="s">
         <v>516</v>
-      </c>
-      <c r="B240" t="s">
-        <v>517</v>
       </c>
       <c r="C240">
         <v>850</v>
@@ -7590,10 +7587,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A241" t="s">
+        <v>517</v>
+      </c>
+      <c r="B241" t="s">
         <v>518</v>
-      </c>
-      <c r="B241" t="s">
-        <v>519</v>
       </c>
       <c r="C241">
         <v>858</v>
@@ -7613,16 +7610,16 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A242" t="s">
+        <v>519</v>
+      </c>
+      <c r="B242" t="s">
         <v>520</v>
-      </c>
-      <c r="B242" t="s">
-        <v>521</v>
       </c>
       <c r="C242">
         <v>860</v>
       </c>
       <c r="D242" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E242" t="s">
         <v>10</v>
@@ -7636,10 +7633,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A243" t="s">
+        <v>521</v>
+      </c>
+      <c r="B243" t="s">
         <v>522</v>
-      </c>
-      <c r="B243" t="s">
-        <v>523</v>
       </c>
       <c r="C243">
         <v>548</v>
@@ -7654,15 +7651,15 @@
         <v>27</v>
       </c>
       <c r="G243" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A244" t="s">
+        <v>523</v>
+      </c>
+      <c r="B244" t="s">
         <v>524</v>
-      </c>
-      <c r="B244" t="s">
-        <v>525</v>
       </c>
       <c r="C244">
         <v>862</v>
@@ -7682,10 +7679,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A245" t="s">
+        <v>525</v>
+      </c>
+      <c r="B245" t="s">
         <v>526</v>
-      </c>
-      <c r="B245" t="s">
-        <v>527</v>
       </c>
       <c r="C245">
         <v>704</v>
@@ -7700,15 +7697,15 @@
         <v>11</v>
       </c>
       <c r="G245" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A246" t="s">
+        <v>527</v>
+      </c>
+      <c r="B246" t="s">
         <v>528</v>
-      </c>
-      <c r="B246" t="s">
-        <v>529</v>
       </c>
       <c r="C246">
         <v>876</v>
@@ -7723,15 +7720,15 @@
         <v>27</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A247" t="s">
+        <v>529</v>
+      </c>
+      <c r="B247" t="s">
         <v>530</v>
-      </c>
-      <c r="B247" t="s">
-        <v>531</v>
       </c>
       <c r="C247">
         <v>732</v>
@@ -7751,10 +7748,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A248" t="s">
+        <v>531</v>
+      </c>
+      <c r="B248" t="s">
         <v>532</v>
-      </c>
-      <c r="B248" t="s">
-        <v>533</v>
       </c>
       <c r="C248">
         <v>887</v>
@@ -7769,15 +7766,15 @@
         <v>11</v>
       </c>
       <c r="G248" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A249" t="s">
+        <v>533</v>
+      </c>
+      <c r="B249" t="s">
         <v>534</v>
-      </c>
-      <c r="B249" t="s">
-        <v>535</v>
       </c>
       <c r="C249">
         <v>894</v>
@@ -7797,10 +7794,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A250" t="s">
+        <v>535</v>
+      </c>
+      <c r="B250" t="s">
         <v>536</v>
-      </c>
-      <c r="B250" t="s">
-        <v>537</v>
       </c>
       <c r="C250">
         <v>716</v>

</xml_diff>